<commit_message>
Add 2 Points and Sliding Window
</commit_message>
<xml_diff>
--- a/Patterns/schedule.xlsx
+++ b/Patterns/schedule.xlsx
@@ -5,34 +5,32 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xtstc131/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xtstc131/Documents/Trail/Leetcode/Patterns/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8D8098-7455-B845-8FD1-2DD4FFDFC856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A297F55-C01D-DA4A-9C33-4C9D6164395F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Task Schedule" sheetId="1" r:id="rId1"/>
     <sheet name="Weekly Task Schedule (2)" sheetId="5" r:id="rId2"/>
-    <sheet name="Task List" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Classes" localSheetId="1">TaskSchedule4[[#All],[Column1]]</definedName>
+    <definedName name="Classes" localSheetId="1">#REF!</definedName>
     <definedName name="Classes">TaskSchedule[[#All],[Column1]]</definedName>
-    <definedName name="ColumnTitle2" localSheetId="1">TaskList[[#Headers],[Date]]</definedName>
-    <definedName name="ColumnTitle2">TaskList[[#Headers],[Date]]</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Task List'!$3:$3</definedName>
+    <definedName name="ColumnTitle2" localSheetId="1">#REF!</definedName>
+    <definedName name="ColumnTitle2">#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Weekly Task Schedule'!$4:$5</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Weekly Task Schedule (2)'!$4:$5</definedName>
     <definedName name="RowTitleRegion1..I3" localSheetId="1">'Weekly Task Schedule (2)'!$H$3</definedName>
     <definedName name="RowTitleRegion1..I3">'Weekly Task Schedule'!$H$3</definedName>
     <definedName name="StartDate" localSheetId="1">'Weekly Task Schedule (2)'!$I$3</definedName>
     <definedName name="StartDate">'Weekly Task Schedule'!$I$3</definedName>
-    <definedName name="Title1" localSheetId="1">TaskSchedule4[[#All],[Column1]]</definedName>
+    <definedName name="Title1" localSheetId="1">#REF!</definedName>
     <definedName name="Title1">TaskSchedule[[#All],[Column1]]</definedName>
-    <definedName name="WhoField" localSheetId="1">TaskList[Class]</definedName>
-    <definedName name="WhoField">TaskList[Class]</definedName>
+    <definedName name="WhoField" localSheetId="1">#REF!</definedName>
+    <definedName name="WhoField">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>TASK SCHEDULE</t>
   </si>
@@ -57,73 +55,10 @@
     <t xml:space="preserve"> Schedule Start Date:</t>
   </si>
   <si>
-    <t>ENG 101</t>
-  </si>
-  <si>
-    <t>ART 101</t>
-  </si>
-  <si>
-    <t>MTH 101</t>
-  </si>
-  <si>
-    <t>LIT 101</t>
-  </si>
-  <si>
-    <t>HIS 101</t>
-  </si>
-  <si>
-    <t>OTHER</t>
-  </si>
-  <si>
-    <t>TASK LIST</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Assignment/Task</t>
-  </si>
-  <si>
-    <t>Match Data</t>
-  </si>
-  <si>
-    <t>Page 90 &amp; review chapter 5 for test on Friday</t>
-  </si>
-  <si>
-    <t>Worksheet 56 (odd only) and study for test on Thursday</t>
-  </si>
-  <si>
-    <t>Prep for Lab</t>
-  </si>
-  <si>
-    <t>Chapter 5 - 8 test</t>
-  </si>
-  <si>
-    <t>Pages 78 - 88 &amp; outline chapter 4</t>
-  </si>
-  <si>
-    <t>Study for test</t>
-  </si>
-  <si>
-    <t>Clean room for inspection</t>
-  </si>
-  <si>
-    <t>Order pizza for study group</t>
-  </si>
-  <si>
-    <t>Outline Essay</t>
-  </si>
-  <si>
     <t>WEEKLY</t>
   </si>
   <si>
     <t>To Task List</t>
-  </si>
-  <si>
-    <t>To Weekly Task Schedule</t>
   </si>
   <si>
     <t>Winter</t>
@@ -133,9 +68,6 @@
   </si>
   <si>
     <t>Revise</t>
-  </si>
-  <si>
-    <t> Sliding window</t>
   </si>
   <si>
     <t>two points</t>
@@ -149,6 +81,15 @@
   <si>
     <t> Cyclic Sort</t>
   </si>
+  <si>
+    <t>Tree Depth First Search </t>
+  </si>
+  <si>
+    <t>Merge Intervals</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cyclic Sort</t>
+  </si>
 </sst>
 </file>
 
@@ -160,7 +101,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3"/>
@@ -251,8 +192,14 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="13.2"/>
+      <color rgb="FF1A1A1A"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,6 +221,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -420,16 +373,16 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="3">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -590,25 +543,25 @@
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="1" dataCellStyle="Normal">
-      <calculatedColumnFormula>IFERROR(INDEX(TaskList[],MATCH(C$5&amp;$B6,TaskList[Match Data],0),3),"")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B6,#REF!,0),3),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3" dataCellStyle="Normal">
-      <calculatedColumnFormula>IFERROR(INDEX(TaskList[],MATCH(D$5&amp;$B6,TaskList[Match Data],0),3),"")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B6,#REF!,0),3),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4" dataCellStyle="Normal">
-      <calculatedColumnFormula>IFERROR(INDEX(TaskList[],MATCH(E$5&amp;$B6,TaskList[Match Data],0),3),"")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B6,#REF!,0),3),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5" dataCellStyle="Normal">
-      <calculatedColumnFormula>IFERROR(INDEX(TaskList[],MATCH(F$5&amp;$B6,TaskList[Match Data],0),3),"")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B6,#REF!,0),3),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6" dataCellStyle="Normal">
-      <calculatedColumnFormula>IFERROR(INDEX(TaskList[],MATCH(G$5&amp;$B6,TaskList[Match Data],0),3),"")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B6,#REF!,0),3),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7" dataCellStyle="Normal">
-      <calculatedColumnFormula>IFERROR(INDEX(TaskList[],MATCH(H$5&amp;$B6,TaskList[Match Data],0),3),"")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B6,#REF!,0),3),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8" dataCellStyle="Normal">
-      <calculatedColumnFormula>IFERROR(INDEX(TaskList[],MATCH(I$5&amp;$B6,TaskList[Match Data],0),3),"")</calculatedColumnFormula>
+      <calculatedColumnFormula>IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B6,#REF!,0),3),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Weekly Task List" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -621,58 +574,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{87DD73EC-39A5-2F41-B0FF-FDA636961329}" name="TaskSchedule4" displayName="TaskSchedule4" ref="B6:I11" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B05C4B53-F460-D248-8624-9C7CA41CB91B}" name="TaskSchedule6" displayName="TaskSchedule6" ref="B6:I11" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{80F473AF-E871-7B42-B114-4852D6198059}" name="Column1" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{292CE1D1-167A-5C4B-8663-F64FABB8D482}" name="Column2" dataDxfId="0" dataCellStyle="Normal">
-      <calculatedColumnFormula>IFERROR(INDEX(TaskList[],MATCH(C$5&amp;$B6,TaskList[Match Data],0),3),"")</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{9FFEF487-934D-8743-9EF2-D17EB03D952F}" name="Column1" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{890CFB0A-F202-D544-8F9F-EF7322751E2B}" name="Column2" dataDxfId="0" dataCellStyle="Normal">
+      <calculatedColumnFormula>IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B6,#REF!,0),3),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D363CACD-D54A-2147-89FE-23869B78BB4C}" name="Column3" dataCellStyle="Normal">
-      <calculatedColumnFormula>IFERROR(INDEX(TaskList[],MATCH(D$5&amp;$B6,TaskList[Match Data],0),3),"")</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{8B52FBED-B8EC-954A-BD09-8F752D7518EF}" name="Column3" dataCellStyle="Normal">
+      <calculatedColumnFormula>IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B6,#REF!,0),3),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9A2E2C20-22E3-C641-BBA3-A9D9FEDC0844}" name="Column4" dataCellStyle="Normal">
-      <calculatedColumnFormula>IFERROR(INDEX(TaskList[],MATCH(E$5&amp;$B6,TaskList[Match Data],0),3),"")</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{41302CB1-7F0B-2A4B-B7B1-500C91BAE773}" name="Column4" dataCellStyle="Normal">
+      <calculatedColumnFormula>IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B6,#REF!,0),3),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FFF1E5C0-9370-9943-88B9-CA794893FE38}" name="Column5" dataCellStyle="Normal">
-      <calculatedColumnFormula>IFERROR(INDEX(TaskList[],MATCH(F$5&amp;$B6,TaskList[Match Data],0),3),"")</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{64A9A496-4B5C-FE47-9CEC-CD27F90ADBBE}" name="Column5" dataCellStyle="Normal">
+      <calculatedColumnFormula>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B6,#REF!,0),3),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7C255EA5-B40B-0140-A14F-ABD289F746BA}" name="Column6" dataCellStyle="Normal">
-      <calculatedColumnFormula>IFERROR(INDEX(TaskList[],MATCH(G$5&amp;$B6,TaskList[Match Data],0),3),"")</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{C5147C6B-146D-CF4F-8401-D64E31EC7161}" name="Column6" dataCellStyle="Normal">
+      <calculatedColumnFormula>IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B6,#REF!,0),3),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4AADF5BA-E6F6-4B49-9423-ADD38B011482}" name="Column7" dataCellStyle="Normal">
-      <calculatedColumnFormula>IFERROR(INDEX(TaskList[],MATCH(H$5&amp;$B6,TaskList[Match Data],0),3),"")</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{40990E8B-F966-4E4A-A720-D1C8839D3E0C}" name="Column7" dataCellStyle="Normal">
+      <calculatedColumnFormula>IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B6,#REF!,0),3),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6792371A-19AB-AA4B-AD94-8A976176488C}" name="Column8" dataCellStyle="Normal">
-      <calculatedColumnFormula>IFERROR(INDEX(TaskList[],MATCH(I$5&amp;$B6,TaskList[Match Data],0),3),"")</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{D0EDBC50-E99D-6845-9C27-8A7D68669225}" name="Column8" dataCellStyle="Normal">
+      <calculatedColumnFormula>IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B6,#REF!,0),3),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Weekly Task List" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
       <x14:table altTextSummary="Enter Class titles in first column of this table &amp; other columns are automatically updated from the Assignment/Tasks entered in Task List worksheet"/>
-    </ext>
-  </extLst>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TaskList" displayName="TaskList" ref="B3:E12" totalsRowShown="0" headerRowCellStyle="Heading 2">
-  <autoFilter ref="B3:E12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:E13">
-    <sortCondition ref="B4:B13"/>
-  </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataCellStyle="Date"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Class" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Assignment/Task" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Match Data">
-      <calculatedColumnFormula>TaskList[[#This Row],[Date]]&amp;TaskList[[#This Row],[Class]]</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="Weekly Task List" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
-      <x14:table altTextSummary="Enter date, class, and assignment or task. Use table filters to find specific entries"/>
     </ext>
   </extLst>
 </table>
@@ -947,7 +877,7 @@
   </sheetPr>
   <dimension ref="B1:I11"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -961,12 +891,12 @@
   <sheetData>
     <row r="1" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="5" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="2:9" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -977,248 +907,232 @@
         <v>1</v>
       </c>
       <c r="I3" s="3">
-        <f ca="1">TODAY()</f>
-        <v>43942</v>
+        <f>DATEVALUE("2020-5-2")</f>
+        <v>43953</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C4" s="9" t="str">
-        <f ca="1">TEXT(WEEKDAY(StartDate),"aaaa")</f>
+        <f>TEXT(WEEKDAY(StartDate),"aaaa")</f>
+        <v>Saturday</v>
+      </c>
+      <c r="D4" s="9" t="str">
+        <f>TEXT(WEEKDAY(StartDate)+1,"aaaa")</f>
+        <v>Sunday</v>
+      </c>
+      <c r="E4" s="9" t="str">
+        <f>TEXT(WEEKDAY(StartDate)+2,"aaaa")</f>
+        <v>Monday</v>
+      </c>
+      <c r="F4" s="9" t="str">
+        <f>TEXT(WEEKDAY(StartDate)+3,"aaaa")</f>
         <v>Tuesday</v>
       </c>
-      <c r="D4" s="9" t="str">
-        <f ca="1">TEXT(WEEKDAY(StartDate)+1,"aaaa")</f>
+      <c r="G4" s="9" t="str">
+        <f>TEXT(WEEKDAY(StartDate)+4,"aaaa")</f>
         <v>Wednesday</v>
       </c>
-      <c r="E4" s="9" t="str">
-        <f ca="1">TEXT(WEEKDAY(StartDate)+2,"aaaa")</f>
+      <c r="H4" s="9" t="str">
+        <f>TEXT(WEEKDAY(StartDate)+5,"aaaa")</f>
         <v>Thursday</v>
       </c>
-      <c r="F4" s="9" t="str">
-        <f ca="1">TEXT(WEEKDAY(StartDate)+3,"aaaa")</f>
+      <c r="I4" s="9" t="str">
+        <f>TEXT(WEEKDAY(StartDate)+6,"aaaa")</f>
         <v>Friday</v>
-      </c>
-      <c r="G4" s="9" t="str">
-        <f ca="1">TEXT(WEEKDAY(StartDate)+4,"aaaa")</f>
-        <v>Saturday</v>
-      </c>
-      <c r="H4" s="9" t="str">
-        <f ca="1">TEXT(WEEKDAY(StartDate)+5,"aaaa")</f>
-        <v>Sunday</v>
-      </c>
-      <c r="I4" s="9" t="str">
-        <f ca="1">TEXT(WEEKDAY(StartDate)+6,"aaaa")</f>
-        <v>Monday</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="8">
-        <f ca="1">YEAR(StartDate)</f>
+        <f>YEAR(StartDate)</f>
         <v>2020</v>
       </c>
       <c r="C5" s="4">
-        <f ca="1">StartDate</f>
-        <v>43942</v>
+        <f>StartDate</f>
+        <v>43953</v>
       </c>
       <c r="D5" s="4">
-        <f ca="1">C5+1</f>
-        <v>43943</v>
+        <f>C5+1</f>
+        <v>43954</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" ref="E5:I5" ca="1" si="0">D5+1</f>
-        <v>43944</v>
+        <f t="shared" ref="E5:F5" si="0">D5+1</f>
+        <v>43955</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>43945</v>
+        <f t="shared" si="0"/>
+        <v>43956</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>43946</v>
+        <f>F5+1</f>
+        <v>43957</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>43947</v>
+        <f>G5+1</f>
+        <v>43958</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>43948</v>
+        <f>H5+1</f>
+        <v>43959</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(C$5&amp;$B6,TaskList[Match Data],0),3),"")</f>
-        <v/>
-      </c>
-      <c r="D6" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(D$5&amp;$B6,TaskList[Match Data],0),3),"")</f>
-        <v/>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>32</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
     </row>
     <row r="7" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(C$5&amp;$B7,TaskList[Match Data],0),3),"")</f>
-        <v/>
-      </c>
-      <c r="D7" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(D$5&amp;$B7,TaskList[Match Data],0),3),"")</f>
-        <v/>
-      </c>
-      <c r="E7" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(E$5&amp;$B7,TaskList[Match Data],0),3),"")</f>
-        <v/>
-      </c>
-      <c r="F7" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(F$5&amp;$B7,TaskList[Match Data],0),3),"")</f>
-        <v/>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>30</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
     </row>
     <row r="8" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(C$5&amp;$B8,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(E$5&amp;$B8,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(F$5&amp;$B8,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(G$5&amp;$B8,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(H$5&amp;$B8,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(I$5&amp;$B8,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(C$5&amp;$B9,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="D9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(D$5&amp;$B9,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(E$5&amp;$B9,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(F$5&amp;$B9,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(G$5&amp;$B9,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(H$5&amp;$B9,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(I$5&amp;$B9,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(C$5&amp;$B10,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="D10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(D$5&amp;$B10,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(E$5&amp;$B10,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(F$5&amp;$B10,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(G$5&amp;$B10,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(H$5&amp;$B10,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(I$5&amp;$B10,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(C$5&amp;$B11,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="D11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(D$5&amp;$B11,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(E$5&amp;$B11,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(F$5&amp;$B11,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(G$5&amp;$B11,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(H$5&amp;$B11,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(I$5&amp;$B11,TaskList[Match Data],0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>
@@ -1258,7 +1172,7 @@
   <dimension ref="B1:I11"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1271,12 +1185,12 @@
   <sheetData>
     <row r="1" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="5" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="2:9" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1288,40 +1202,40 @@
       </c>
       <c r="I3" s="3">
         <f ca="1">TODAY()+6</f>
-        <v>43948</v>
+        <v>43959</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C4" s="9" t="str">
         <f ca="1">TEXT(WEEKDAY(StartDate),"aaaa")</f>
-        <v>Monday</v>
+        <v>Friday</v>
       </c>
       <c r="D4" s="9" t="str">
         <f ca="1">TEXT(WEEKDAY(StartDate)+1,"aaaa")</f>
-        <v>Tuesday</v>
+        <v>Saturday</v>
       </c>
       <c r="E4" s="9" t="str">
         <f ca="1">TEXT(WEEKDAY(StartDate)+2,"aaaa")</f>
-        <v>Wednesday</v>
+        <v>Sunday</v>
       </c>
       <c r="F4" s="9" t="str">
         <f ca="1">TEXT(WEEKDAY(StartDate)+3,"aaaa")</f>
-        <v>Thursday</v>
+        <v>Monday</v>
       </c>
       <c r="G4" s="9" t="str">
         <f ca="1">TEXT(WEEKDAY(StartDate)+4,"aaaa")</f>
-        <v>Friday</v>
+        <v>Tuesday</v>
       </c>
       <c r="H4" s="9" t="str">
         <f ca="1">TEXT(WEEKDAY(StartDate)+5,"aaaa")</f>
-        <v>Saturday</v>
+        <v>Wednesday</v>
       </c>
       <c r="I4" s="9" t="str">
         <f ca="1">TEXT(WEEKDAY(StartDate)+6,"aaaa")</f>
-        <v>Sunday</v>
+        <v>Thursday</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1331,213 +1245,189 @@
       </c>
       <c r="C5" s="4">
         <f ca="1">StartDate</f>
-        <v>43948</v>
+        <v>43959</v>
       </c>
       <c r="D5" s="4">
         <f ca="1">C5+1</f>
-        <v>43949</v>
+        <v>43960</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" ref="E5:I5" ca="1" si="0">D5+1</f>
-        <v>43950</v>
+        <f t="shared" ref="E5:F5" ca="1" si="0">D5+1</f>
+        <v>43961</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>43951</v>
+        <v>43962</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>43952</v>
+        <f ca="1">F5+1</f>
+        <v>43963</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>43953</v>
+        <f ca="1">G5+1</f>
+        <v>43964</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>43954</v>
+        <f ca="1">H5+1</f>
+        <v>43965</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(C$5&amp;$B6,TaskList[Match Data],0),3),"")</f>
-        <v/>
-      </c>
-      <c r="D6" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(D$5&amp;$B6,TaskList[Match Data],0),3),"")</f>
-        <v/>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>32</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
     </row>
     <row r="7" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(C$5&amp;$B7,TaskList[Match Data],0),3),"")</f>
-        <v/>
-      </c>
-      <c r="D7" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(D$5&amp;$B7,TaskList[Match Data],0),3),"")</f>
-        <v/>
-      </c>
-      <c r="E7" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(E$5&amp;$B7,TaskList[Match Data],0),3),"")</f>
-        <v/>
-      </c>
-      <c r="F7" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(F$5&amp;$B7,TaskList[Match Data],0),3),"")</f>
-        <v/>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>30</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
     </row>
     <row r="8" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(C$5&amp;$B8,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(E$5&amp;$B8,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(F$5&amp;$B8,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(G$5&amp;$B8,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(H$5&amp;$B8,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(I$5&amp;$B8,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(C$5&amp;$B9,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="D9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(D$5&amp;$B9,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(E$5&amp;$B9,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(F$5&amp;$B9,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(G$5&amp;$B9,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(H$5&amp;$B9,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(I$5&amp;$B9,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(C$5&amp;$B10,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="D10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(D$5&amp;$B10,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(E$5&amp;$B10,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(F$5&amp;$B10,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(G$5&amp;$B10,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(H$5&amp;$B10,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(I$5&amp;$B10,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(C$5&amp;$B11,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="D11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(D$5&amp;$B11,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(E$5&amp;$B11,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(F$5&amp;$B11,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(G$5&amp;$B11,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(H$5&amp;$B11,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(TaskList[],MATCH(I$5&amp;$B11,TaskList[Match Data],0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <dataValidations count="9">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cells C5 to I5 contain ascending dates for each day of the week starting with Start Date. Tasks are automatically updated under each column for each entry in the left column" sqref="C5" xr:uid="{6FD79899-90AE-624A-BE33-7961B8127AEA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cells C4 to I4 contains weekdays. The starting day of the week in this cell is automatically updated based on Schedule Start Date. To change this weekday, enter new date in cell I3" sqref="C4" xr:uid="{F567E6D8-836F-3D43-B4A4-15627D0513D3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a category name for this task schedule in this cell" sqref="B4" xr:uid="{0B2211DE-08A3-B047-A760-0C160EC829D6}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Start Date Year from cell I3. Enter Class titles in this column under this heading. Corresponding tasks are automatically updated from Task List worksheet" sqref="B5" xr:uid="{8B010980-E81E-454D-9560-4CDB796646A2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cells C5 to I5 contain ascending dates for each day of the week starting with Start Date. Tasks are automatically updated under each column for each entry in the left column" sqref="C5" xr:uid="{8320A299-60E0-2B4B-B4E9-FCE8247579E2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cells C4 to I4 contains weekdays. The starting day of the week in this cell is automatically updated based on Schedule Start Date. To change this weekday, enter new date in cell I3" sqref="C4" xr:uid="{0776413C-9790-D041-9B76-D2CFB7C545EA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a category name for this task schedule in this cell" sqref="B4" xr:uid="{961965C4-D360-4F41-BA90-6A702769706E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Start Date Year from cell I3. Enter Class titles in this column under this heading. Corresponding tasks are automatically updated from Task List worksheet" sqref="B5" xr:uid="{A3C41B45-7103-8B41-B6FF-73EE1F4DFA06}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Schedule Start Date in this cell. Task Schedule table will automatically update for the week starting at this date" sqref="I3" xr:uid="{CF955B55-399D-E24B-8349-55C9A044789C}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Schedule Start Date in cell at right" sqref="H3" xr:uid="{36005265-075F-304B-8717-D481CBD86AC3}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the worksheet is in cells B2 &amp; B3. Enter Schedule Start Date in cell I3" sqref="B2" xr:uid="{0082A4C1-0E86-9A4C-B63E-1A5F6D8B3834}"/>
@@ -1557,221 +1447,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <tabColor theme="4" tint="0.79998168889431442"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="B1:E12"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="60.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="10">
-        <f ca="1">TODAY()</f>
-        <v>43942</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="11" t="str">
-        <f ca="1">TaskList[[#This Row],[Date]]&amp;TaskList[[#This Row],[Class]]</f>
-        <v>43942HIS 101</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="10">
-        <f ca="1">TODAY()+1</f>
-        <v>43943</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="11" t="str">
-        <f ca="1">TaskList[[#This Row],[Date]]&amp;TaskList[[#This Row],[Class]]</f>
-        <v>43943MTH 101</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="10">
-        <f ca="1">TODAY()+2</f>
-        <v>43944</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="11" t="str">
-        <f ca="1">TaskList[[#This Row],[Date]]&amp;TaskList[[#This Row],[Class]]</f>
-        <v>43944ART 101</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="10">
-        <f ca="1">TODAY()+3</f>
-        <v>43945</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="12" t="str">
-        <f ca="1">TaskList[[#This Row],[Date]]&amp;TaskList[[#This Row],[Class]]</f>
-        <v>43945HIS 101</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="10">
-        <f ca="1">TODAY()+4</f>
-        <v>43946</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="11" t="str">
-        <f ca="1">TaskList[[#This Row],[Date]]&amp;TaskList[[#This Row],[Class]]</f>
-        <v>43946LIT 101</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="10">
-        <f ca="1">TODAY()+4</f>
-        <v>43946</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="11" t="str">
-        <f ca="1">TaskList[[#This Row],[Date]]&amp;TaskList[[#This Row],[Class]]</f>
-        <v>43946HIS 101</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="10">
-        <f ca="1">TODAY()+5</f>
-        <v>43947</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="12" t="str">
-        <f ca="1">TaskList[[#This Row],[Date]]&amp;TaskList[[#This Row],[Class]]</f>
-        <v>43947OTHER</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="10">
-        <f ca="1">TODAY()+5</f>
-        <v>43947</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="12" t="str">
-        <f ca="1">TaskList[[#This Row],[Date]]&amp;TaskList[[#This Row],[Class]]</f>
-        <v>43947OTHER</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="10">
-        <f ca="1">TODAY()+6</f>
-        <v>43948</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="11" t="str">
-        <f ca="1">TaskList[[#This Row],[Date]]&amp;TaskList[[#This Row],[Class]]</f>
-        <v>43948ENG 101</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataConsolidate/>
-  <dataValidations count="7">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create Task List in this worksheet. Tasks will automatically update in Task Schedule table. Select B1 to navigate back to Weekly Task Schedule worksheet" sqref="A1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigational link to Weekly Task Schedule worksheet" sqref="B1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the worksheet is in this cell. Enter task details in table below" sqref="B2" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter date in this column under this heading. Use heading filters to find specific entries" sqref="B3" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Class in this column under this heading. Class list is updated from Task Schedule table column B. Press ALT+DOWN arrow to open drop down list, then ENTER to make selection" sqref="C3" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Assignment or Task for the corresponding class in column C, in this column under this heading" sqref="D3" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Entry doesn't match items in the list. Select No, then press ALT+DOWN ARROW and ENTER to select a new entry, CANCEL to clear the selection" sqref="C4:C12" xr:uid="{00000000-0002-0000-0100-000006000000}">
-      <formula1>Classes</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B1" location="'Weekly Task Schedule'!A1" tooltip="Select to view Weekly Task Schedule worksheet" display="To Weekly Task Schedule" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-  </hyperlinks>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="76" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <headerFooter differentFirst="1">
-    <oddFooter>Page &amp;P of &amp;N</oddFooter>
-  </headerFooter>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Move odd code into DataStructure folder
</commit_message>
<xml_diff>
--- a/Patterns/schedule.xlsx
+++ b/Patterns/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xtstc131/Documents/Trail/Leetcode/Patterns/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A297F55-C01D-DA4A-9C33-4C9D6164395F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D79D97E-6B00-D34B-9B82-4CF2ED1C9257}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Task Schedule" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>TASK SCHEDULE</t>
   </si>
@@ -79,16 +79,40 @@
     <t>Tree Breadth First Search</t>
   </si>
   <si>
-    <t> Cyclic Sort</t>
-  </si>
-  <si>
     <t>Tree Depth First Search </t>
   </si>
   <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>Merge Intervals</t>
   </si>
   <si>
-    <t xml:space="preserve"> Cyclic Sort</t>
+    <t>Cyclic Sort</t>
+  </si>
+  <si>
+    <t>In-place Reversal of a LinkedList</t>
+  </si>
+  <si>
+    <t>Two Heaps</t>
+  </si>
+  <si>
+    <t>Subsets</t>
+  </si>
+  <si>
+    <t>Modified Binary Search</t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
+  <si>
+    <t>DFS</t>
   </si>
 </sst>
 </file>
@@ -199,7 +223,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +250,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -342,7 +378,7 @@
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -379,10 +415,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="9" fontId="12" fillId="7" borderId="0" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="7" borderId="0" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -877,8 +925,8 @@
   </sheetPr>
   <dimension ref="B1:I11"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" showZeros="0" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -898,6 +946,9 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="2:9" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
@@ -982,42 +1033,46 @@
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="12" t="s">
+      <c r="E6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
     </row>
     <row r="7" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="11"/>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="11"/>
+      <c r="F7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="I7" s="11"/>
     </row>
     <row r="8" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1033,9 +1088,8 @@
         <f>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
-      <c r="G8" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B8,#REF!,0),3),"")</f>
-        <v/>
+      <c r="G8" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H8" s="1" t="str">
         <f>IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B8,#REF!,0),3),"")</f>
@@ -1055,10 +1109,6 @@
         <f>IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
-      <c r="E9" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B9,#REF!,0),3),"")</f>
-        <v/>
-      </c>
       <c r="F9" s="1" t="str">
         <f>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
@@ -1137,7 +1187,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="9">
+  <dataValidations count="9">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Track Weekly Tasks in this Weekly Task Schedule worksheet. Add tasks in Task List worksheet to automatically update the schedule. Select cell B1 to navigate to Task List worksheet" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to Task List worksheet" sqref="B1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the worksheet is in cells B2 &amp; B3. Enter Schedule Start Date in cell I3" sqref="B2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
@@ -1171,8 +1221,8 @@
   </sheetPr>
   <dimension ref="B1:I11"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1201,8 +1251,8 @@
         <v>1</v>
       </c>
       <c r="I3" s="3">
-        <f ca="1">TODAY()+6</f>
-        <v>43959</v>
+        <f>DATEVALUE("2020-5-11")</f>
+        <v>43962</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1210,215 +1260,231 @@
         <v>4</v>
       </c>
       <c r="C4" s="9" t="str">
-        <f ca="1">TEXT(WEEKDAY(StartDate),"aaaa")</f>
+        <f>TEXT(WEEKDAY(StartDate),"aaaa")</f>
+        <v>Monday</v>
+      </c>
+      <c r="D4" s="9" t="str">
+        <f>TEXT(WEEKDAY(StartDate)+1,"aaaa")</f>
+        <v>Tuesday</v>
+      </c>
+      <c r="E4" s="9" t="str">
+        <f>TEXT(WEEKDAY(StartDate)+2,"aaaa")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="F4" s="9" t="str">
+        <f>TEXT(WEEKDAY(StartDate)+3,"aaaa")</f>
+        <v>Thursday</v>
+      </c>
+      <c r="G4" s="9" t="str">
+        <f>TEXT(WEEKDAY(StartDate)+4,"aaaa")</f>
         <v>Friday</v>
       </c>
-      <c r="D4" s="9" t="str">
-        <f ca="1">TEXT(WEEKDAY(StartDate)+1,"aaaa")</f>
+      <c r="H4" s="9" t="str">
+        <f>TEXT(WEEKDAY(StartDate)+5,"aaaa")</f>
         <v>Saturday</v>
       </c>
-      <c r="E4" s="9" t="str">
-        <f ca="1">TEXT(WEEKDAY(StartDate)+2,"aaaa")</f>
+      <c r="I4" s="9" t="str">
+        <f>TEXT(WEEKDAY(StartDate)+6,"aaaa")</f>
         <v>Sunday</v>
-      </c>
-      <c r="F4" s="9" t="str">
-        <f ca="1">TEXT(WEEKDAY(StartDate)+3,"aaaa")</f>
-        <v>Monday</v>
-      </c>
-      <c r="G4" s="9" t="str">
-        <f ca="1">TEXT(WEEKDAY(StartDate)+4,"aaaa")</f>
-        <v>Tuesday</v>
-      </c>
-      <c r="H4" s="9" t="str">
-        <f ca="1">TEXT(WEEKDAY(StartDate)+5,"aaaa")</f>
-        <v>Wednesday</v>
-      </c>
-      <c r="I4" s="9" t="str">
-        <f ca="1">TEXT(WEEKDAY(StartDate)+6,"aaaa")</f>
-        <v>Thursday</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="8">
-        <f ca="1">YEAR(StartDate)</f>
+        <f>YEAR(StartDate)</f>
         <v>2020</v>
       </c>
       <c r="C5" s="4">
-        <f ca="1">StartDate</f>
-        <v>43959</v>
+        <f>StartDate</f>
+        <v>43962</v>
       </c>
       <c r="D5" s="4">
-        <f ca="1">C5+1</f>
-        <v>43960</v>
+        <f>C5+1</f>
+        <v>43963</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" ref="E5:F5" ca="1" si="0">D5+1</f>
-        <v>43961</v>
+        <f t="shared" ref="E5:F5" si="0">D5+1</f>
+        <v>43964</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>43962</v>
+        <f t="shared" si="0"/>
+        <v>43965</v>
       </c>
       <c r="G5" s="4">
-        <f ca="1">F5+1</f>
-        <v>43963</v>
+        <f>F5+1</f>
+        <v>43966</v>
       </c>
       <c r="H5" s="4">
-        <f ca="1">G5+1</f>
-        <v>43964</v>
+        <f>G5+1</f>
+        <v>43967</v>
       </c>
       <c r="I5" s="4">
-        <f ca="1">H5+1</f>
-        <v>43965</v>
+        <f>H5+1</f>
+        <v>43968</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="C6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="I6" s="11"/>
     </row>
     <row r="7" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>7</v>
+      <c r="C7" s="16" t="s">
+        <v>20</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+        <v>21</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B8,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B8,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B8,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B8,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B8,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I8" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B8,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B9,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="D9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B9,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B9,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B9,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B9,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B9,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I9" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B9,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B10,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="D10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B10,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B10,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B10,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B10,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B10,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I10" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B10,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B11,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="D11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B11,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B11,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B11,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B11,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B11,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I11" s="1" t="str">
-        <f ca="1">IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B11,#REF!,0),3),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
A long overdue update
</commit_message>
<xml_diff>
--- a/Patterns/schedule.xlsx
+++ b/Patterns/schedule.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xtstc131/Documents/Trail/Leetcode/Patterns/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E29085B-28BA-A246-8493-24A596154ECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E7907C-E947-F74B-AFE4-F3B50C632EFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Task Schedule" sheetId="1" r:id="rId1"/>
     <sheet name="Weekly Task Schedule (2)" sheetId="5" r:id="rId2"/>
     <sheet name="Weekly Task Schedule (3)" sheetId="7" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="Revise" sheetId="8" r:id="rId4"/>
+    <sheet name="New" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Classes" localSheetId="1">#REF!</definedName>
@@ -49,14 +51,37 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
   <si>
     <t>TASK SCHEDULE</t>
   </si>
@@ -131,6 +156,39 @@
   </si>
   <si>
     <t>Graphs</t>
+  </si>
+  <si>
+    <t>3 new problems</t>
+  </si>
+  <si>
+    <t>5 old problems</t>
+  </si>
+  <si>
+    <t>Slidling Windows</t>
+  </si>
+  <si>
+    <t>Two Points</t>
+  </si>
+  <si>
+    <t>Merge Interval</t>
+  </si>
+  <si>
+    <t>2 Heaps</t>
+  </si>
+  <si>
+    <t>Top K</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>K Way Merge</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>305 （lint:434）</t>
   </si>
 </sst>
 </file>
@@ -143,7 +201,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3"/>
@@ -245,8 +303,63 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="3"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF212121"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF212121"/>
+      <name val="PingFang SC"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,8 +401,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -358,6 +507,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -401,7 +627,7 @@
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -463,6 +689,111 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1291,9 +1622,7 @@
   </sheetPr>
   <dimension ref="B1:I11"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView showGridLines="0" showZeros="0" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1320,76 +1649,76 @@
       <c r="H3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="3">
-        <f>DATEVALUE("2020-5-11")</f>
-        <v>43962</v>
+      <c r="I3" s="3" t="e" cm="1">
+        <f t="array" aca="1" ref="I3" ca="1">New!A1DATEVALUE("2020-5-11")</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9" t="str">
-        <f>TEXT(WEEKDAY(StartDate),"aaaa")</f>
-        <v>Monday</v>
-      </c>
-      <c r="D4" s="9" t="str">
-        <f>TEXT(WEEKDAY(StartDate)+1,"aaaa")</f>
-        <v>Tuesday</v>
-      </c>
-      <c r="E4" s="9" t="str">
-        <f>TEXT(WEEKDAY(StartDate)+2,"aaaa")</f>
-        <v>Wednesday</v>
-      </c>
-      <c r="F4" s="9" t="str">
-        <f>TEXT(WEEKDAY(StartDate)+3,"aaaa")</f>
-        <v>Thursday</v>
-      </c>
-      <c r="G4" s="9" t="str">
-        <f>TEXT(WEEKDAY(StartDate)+4,"aaaa")</f>
-        <v>Friday</v>
-      </c>
-      <c r="H4" s="9" t="str">
-        <f>TEXT(WEEKDAY(StartDate)+5,"aaaa")</f>
-        <v>Saturday</v>
-      </c>
-      <c r="I4" s="9" t="str">
-        <f>TEXT(WEEKDAY(StartDate)+6,"aaaa")</f>
-        <v>Sunday</v>
+      <c r="C4" s="9" t="e">
+        <f ca="1">TEXT(WEEKDAY(StartDate),"aaaa")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D4" s="9" t="e">
+        <f ca="1">TEXT(WEEKDAY(StartDate)+1,"aaaa")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E4" s="9" t="e">
+        <f ca="1">TEXT(WEEKDAY(StartDate)+2,"aaaa")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F4" s="9" t="e">
+        <f ca="1">TEXT(WEEKDAY(StartDate)+3,"aaaa")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G4" s="9" t="e">
+        <f ca="1">TEXT(WEEKDAY(StartDate)+4,"aaaa")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H4" s="9" t="e">
+        <f ca="1">TEXT(WEEKDAY(StartDate)+5,"aaaa")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="I4" s="9" t="e">
+        <f ca="1">TEXT(WEEKDAY(StartDate)+6,"aaaa")</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="8">
-        <f>YEAR(StartDate)</f>
-        <v>2020</v>
-      </c>
-      <c r="C5" s="4">
-        <f>StartDate</f>
-        <v>43962</v>
-      </c>
-      <c r="D5" s="4">
-        <f>C5+1</f>
-        <v>43963</v>
-      </c>
-      <c r="E5" s="4">
-        <f t="shared" ref="E5:F5" si="0">D5+1</f>
-        <v>43964</v>
-      </c>
-      <c r="F5" s="4">
-        <f t="shared" si="0"/>
-        <v>43965</v>
-      </c>
-      <c r="G5" s="4">
-        <f>F5+1</f>
-        <v>43966</v>
-      </c>
-      <c r="H5" s="4">
-        <f>G5+1</f>
-        <v>43967</v>
-      </c>
-      <c r="I5" s="4">
-        <f>H5+1</f>
-        <v>43968</v>
+      <c r="B5" s="8" t="e">
+        <f ca="1">YEAR(StartDate)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C5" s="4" t="e">
+        <f ca="1">StartDate</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D5" s="4" t="e">
+        <f ca="1">C5+1</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E5" s="4" t="e">
+        <f t="shared" ref="E5:F5" ca="1" si="0">D5+1</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F5" s="4" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="G5" s="4" t="e">
+        <f ca="1">F5+1</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H5" s="4" t="e">
+        <f ca="1">G5+1</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="I5" s="4" t="e">
+        <f ca="1">H5+1</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1444,117 +1773,117 @@
     </row>
     <row r="8" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B8,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E8" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B8,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F8" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B8,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G8" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B8,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H8" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B8,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I8" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B8,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B8,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B9,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="D9" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B9,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E9" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B9,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F9" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B9,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G9" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B9,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H9" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B9,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I9" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B9,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B9,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B10,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="D10" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B10,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E10" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B10,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F10" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B10,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G10" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B10,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H10" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B10,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I10" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B10,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B10,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B11,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(C$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="D11" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B11,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(D$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="E11" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B11,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(E$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="F11" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B11,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(F$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="G11" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B11,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(G$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="H11" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B11,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(H$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
       <c r="I11" s="1" t="str">
-        <f>IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B11,#REF!,0),3),"")</f>
+        <f ca="1">IFERROR(INDEX(#REF!,MATCH(I$5&amp;$B11,#REF!,0),3),"")</f>
         <v/>
       </c>
     </row>
@@ -1593,8 +1922,8 @@
   </sheetPr>
   <dimension ref="B1:I11"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" showZeros="0" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1623,8 +1952,8 @@
         <v>1</v>
       </c>
       <c r="I3" s="3">
-        <f>DATEVALUE("2020-6-15")</f>
-        <v>43997</v>
+        <f>DATEVALUE("2020-7-6")</f>
+        <v>44018</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1667,31 +1996,31 @@
       </c>
       <c r="C5" s="4">
         <f>StartDate</f>
-        <v>43997</v>
+        <v>44018</v>
       </c>
       <c r="D5" s="4">
         <f>C5+1</f>
-        <v>43998</v>
+        <v>44019</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" ref="E5:F5" si="0">D5+1</f>
-        <v>43999</v>
+        <v>44020</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" si="0"/>
-        <v>44000</v>
+        <v>44021</v>
       </c>
       <c r="G5" s="4">
         <f>F5+1</f>
-        <v>44001</v>
+        <v>44022</v>
       </c>
       <c r="H5" s="4">
         <f>G5+1</f>
-        <v>44002</v>
+        <v>44023</v>
       </c>
       <c r="I5" s="4">
         <f>H5+1</f>
-        <v>44003</v>
+        <v>44024</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1699,7 +2028,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>22</v>
@@ -1721,7 +2050,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>20</v>
@@ -1885,10 +2214,1055 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01FB1504-426F-3F45-95CA-F46FF13D49CC}">
+  <dimension ref="A1:G137"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78:B82"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="21">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21">
+        <v>3</v>
+      </c>
+      <c r="E1" s="21">
+        <v>4</v>
+      </c>
+      <c r="F1" s="21">
+        <v>5</v>
+      </c>
+      <c r="G1" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
+    </row>
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="22">
+        <v>3</v>
+      </c>
+      <c r="B3" s="23"/>
+    </row>
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="22">
+        <v>76</v>
+      </c>
+      <c r="B4" s="24"/>
+    </row>
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="22">
+        <v>424</v>
+      </c>
+      <c r="B5" s="24"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="22">
+        <v>438</v>
+      </c>
+      <c r="B6" s="24"/>
+    </row>
+    <row r="7" spans="1:7" s="48" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="46">
+        <v>567</v>
+      </c>
+      <c r="B7" s="47"/>
+    </row>
+    <row r="8" spans="1:7" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
+    </row>
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="22">
+        <v>11</v>
+      </c>
+      <c r="B9" s="24"/>
+    </row>
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="22">
+        <v>15</v>
+      </c>
+      <c r="B10" s="24"/>
+    </row>
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="22">
+        <v>16</v>
+      </c>
+      <c r="B11" s="24"/>
+    </row>
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="22">
+        <v>17</v>
+      </c>
+      <c r="B12" s="23"/>
+    </row>
+    <row r="13" spans="1:7" s="48" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="46">
+        <v>42</v>
+      </c>
+      <c r="B13" s="47"/>
+    </row>
+    <row r="14" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="22">
+        <v>75</v>
+      </c>
+      <c r="B14" s="23"/>
+    </row>
+    <row r="15" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22">
+        <v>977</v>
+      </c>
+      <c r="B15" s="24"/>
+    </row>
+    <row r="16" spans="1:7" ht="45" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="39"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33"/>
+    </row>
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="22">
+        <v>2</v>
+      </c>
+      <c r="B17" s="24"/>
+    </row>
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="22">
+        <v>19</v>
+      </c>
+      <c r="B18" s="23"/>
+    </row>
+    <row r="19" spans="1:5" s="48" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="46">
+        <v>83</v>
+      </c>
+      <c r="B19" s="49"/>
+    </row>
+    <row r="20" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="22">
+        <v>141</v>
+      </c>
+      <c r="B20" s="24"/>
+    </row>
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="22">
+        <v>142</v>
+      </c>
+      <c r="B21" s="24"/>
+    </row>
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="22">
+        <v>143</v>
+      </c>
+      <c r="B22" s="23"/>
+    </row>
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="22">
+        <v>148</v>
+      </c>
+      <c r="B23" s="35"/>
+    </row>
+    <row r="24" spans="1:5" s="48" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="46">
+        <v>203</v>
+      </c>
+      <c r="B24" s="47"/>
+    </row>
+    <row r="25" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="22">
+        <v>234</v>
+      </c>
+      <c r="B25" s="38"/>
+    </row>
+    <row r="26" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="22">
+        <v>876</v>
+      </c>
+      <c r="B26" s="24"/>
+    </row>
+    <row r="27" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="40"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="31"/>
+    </row>
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="22">
+        <v>102</v>
+      </c>
+      <c r="B28" s="24"/>
+    </row>
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="22">
+        <v>103</v>
+      </c>
+      <c r="B29" s="24"/>
+    </row>
+    <row r="30" spans="1:5" s="48" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="46">
+        <v>107</v>
+      </c>
+      <c r="B30" s="47"/>
+    </row>
+    <row r="31" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="22">
+        <v>111</v>
+      </c>
+      <c r="B31" s="24"/>
+    </row>
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="22">
+        <v>116</v>
+      </c>
+      <c r="B32" s="24"/>
+    </row>
+    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="22">
+        <v>117</v>
+      </c>
+      <c r="B33" s="35"/>
+      <c r="D33" s="45"/>
+    </row>
+    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="22">
+        <v>199</v>
+      </c>
+      <c r="B34" s="24"/>
+    </row>
+    <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="22">
+        <v>200</v>
+      </c>
+      <c r="B35" s="24"/>
+    </row>
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="22">
+        <v>297</v>
+      </c>
+      <c r="B36" s="23"/>
+    </row>
+    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="22">
+        <v>637</v>
+      </c>
+      <c r="B37" s="24"/>
+    </row>
+    <row r="38" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="22">
+        <v>863</v>
+      </c>
+      <c r="B38" s="35"/>
+    </row>
+    <row r="39" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="31"/>
+    </row>
+    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="22">
+        <v>98</v>
+      </c>
+      <c r="B40" s="35"/>
+    </row>
+    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="22">
+        <v>100</v>
+      </c>
+      <c r="B41" s="24"/>
+    </row>
+    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="22">
+        <v>101</v>
+      </c>
+      <c r="B42" s="24"/>
+    </row>
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="22">
+        <v>104</v>
+      </c>
+      <c r="B43" s="24"/>
+    </row>
+    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="22">
+        <v>105</v>
+      </c>
+      <c r="B44" s="24"/>
+    </row>
+    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="22">
+        <v>106</v>
+      </c>
+      <c r="B45" s="24"/>
+    </row>
+    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="22">
+        <v>108</v>
+      </c>
+      <c r="B46" s="24"/>
+    </row>
+    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="22">
+        <v>109</v>
+      </c>
+      <c r="B47" s="24"/>
+    </row>
+    <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="22">
+        <v>110</v>
+      </c>
+      <c r="B48" s="24"/>
+    </row>
+    <row r="49" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="22">
+        <v>111</v>
+      </c>
+      <c r="B49" s="24"/>
+    </row>
+    <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="22">
+        <v>112</v>
+      </c>
+      <c r="B50" s="24"/>
+    </row>
+    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="22">
+        <v>113</v>
+      </c>
+      <c r="B51" s="24"/>
+    </row>
+    <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="22">
+        <v>114</v>
+      </c>
+      <c r="B52" s="35"/>
+    </row>
+    <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="22">
+        <v>116</v>
+      </c>
+      <c r="B53" s="24"/>
+    </row>
+    <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="22">
+        <v>117</v>
+      </c>
+      <c r="B54" s="24"/>
+    </row>
+    <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="22">
+        <v>124</v>
+      </c>
+      <c r="B55" s="35"/>
+    </row>
+    <row r="56" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="22">
+        <v>129</v>
+      </c>
+      <c r="B56" s="24"/>
+    </row>
+    <row r="57" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="22">
+        <v>130</v>
+      </c>
+      <c r="B57" s="24"/>
+    </row>
+    <row r="58" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="22">
+        <v>199</v>
+      </c>
+      <c r="B58" s="24"/>
+    </row>
+    <row r="59" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="22">
+        <v>200</v>
+      </c>
+      <c r="B59" s="24"/>
+    </row>
+    <row r="60" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="22">
+        <v>207</v>
+      </c>
+      <c r="B60" s="24"/>
+    </row>
+    <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="22">
+        <v>210</v>
+      </c>
+      <c r="B61" s="24"/>
+    </row>
+    <row r="62" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="22">
+        <v>257</v>
+      </c>
+      <c r="B62" s="24"/>
+    </row>
+    <row r="63" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="22">
+        <v>332</v>
+      </c>
+      <c r="B63" s="24"/>
+    </row>
+    <row r="64" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="22">
+        <v>337</v>
+      </c>
+      <c r="B64" s="24"/>
+    </row>
+    <row r="65" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="22">
+        <v>494</v>
+      </c>
+      <c r="B65" s="54"/>
+    </row>
+    <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="22">
+        <v>542</v>
+      </c>
+      <c r="B66" s="24"/>
+    </row>
+    <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="22">
+        <v>695</v>
+      </c>
+      <c r="B67" s="24"/>
+    </row>
+    <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="22">
+        <v>733</v>
+      </c>
+      <c r="B68" s="24"/>
+    </row>
+    <row r="69" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="22">
+        <v>863</v>
+      </c>
+      <c r="B69" s="24"/>
+    </row>
+    <row r="70" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="22">
+        <v>886</v>
+      </c>
+      <c r="B70" s="24"/>
+    </row>
+    <row r="71" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" s="30"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="31"/>
+    </row>
+    <row r="72" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="22">
+        <v>207</v>
+      </c>
+      <c r="B72" s="24"/>
+    </row>
+    <row r="73" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A73" s="22">
+        <v>210</v>
+      </c>
+      <c r="B73" s="24"/>
+    </row>
+    <row r="74" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74" s="22">
+        <v>332</v>
+      </c>
+      <c r="B74" s="24"/>
+    </row>
+    <row r="75" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A75" s="22">
+        <v>997</v>
+      </c>
+      <c r="B75" s="24"/>
+    </row>
+    <row r="76" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="22">
+        <v>1192</v>
+      </c>
+      <c r="B76" s="24"/>
+    </row>
+    <row r="77" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B77" s="30"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="31"/>
+    </row>
+    <row r="78" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" s="22">
+        <v>56</v>
+      </c>
+      <c r="B78" s="55"/>
+    </row>
+    <row r="79" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A79" s="22">
+        <v>57</v>
+      </c>
+      <c r="B79" s="55"/>
+    </row>
+    <row r="80" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" s="22">
+        <v>435</v>
+      </c>
+      <c r="B80" s="55"/>
+    </row>
+    <row r="81" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A81" s="22">
+        <v>452</v>
+      </c>
+      <c r="B81" s="55"/>
+    </row>
+    <row r="82" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="22">
+        <v>986</v>
+      </c>
+      <c r="B82" s="55"/>
+    </row>
+    <row r="83" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B83" s="30"/>
+      <c r="C83" s="30"/>
+      <c r="D83" s="30"/>
+      <c r="E83" s="31"/>
+    </row>
+    <row r="84" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A84" s="22">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A85" s="22">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="22">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B87" s="30"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="31"/>
+    </row>
+    <row r="88" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A88" s="22">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" s="22">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="22">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" s="22">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" s="22">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" s="22">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="22">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A95" s="22">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A96" s="22">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B98" s="30"/>
+      <c r="C98" s="30"/>
+      <c r="D98" s="30"/>
+      <c r="E98" s="31"/>
+    </row>
+    <row r="99" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A99" s="22">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A100" s="22">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A101" s="22">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A102" s="22">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A103" s="22">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A104" s="22">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A105" s="22">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A106" s="22">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="22">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B108" s="30"/>
+      <c r="C108" s="30"/>
+      <c r="D108" s="30"/>
+      <c r="E108" s="31"/>
+    </row>
+    <row r="109" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A109" s="22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A110" s="22">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A111" s="22">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A112" s="22">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="22">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B114" s="30"/>
+      <c r="C114" s="30"/>
+      <c r="D114" s="30"/>
+      <c r="E114" s="31"/>
+    </row>
+    <row r="115" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A115" s="22">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A116" s="22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A117" s="22">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A118" s="22">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A119" s="22">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A120" s="22">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B122" s="30"/>
+      <c r="C122" s="30"/>
+      <c r="D122" s="30"/>
+      <c r="E122" s="31"/>
+    </row>
+    <row r="123" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A123" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A124" s="22">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A125" s="22">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A126" s="22">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A127" s="22">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A128" s="22">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A129" s="22">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A130" s="22">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A131" s="22">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A132" s="22">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A133" s="22">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A134" s="22">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A135" s="22">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A136" s="22">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A137" s="22">
+        <v>518</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03DF64C-CE01-984C-B495-735206B43DD7}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="21"/>
+    <col min="4" max="4" width="10.83203125" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="25">
+        <v>44018</v>
+      </c>
+      <c r="B1" s="26">
+        <v>134</v>
+      </c>
+      <c r="C1" s="28">
+        <v>135</v>
+      </c>
+      <c r="D1" s="26">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="25">
+        <v>44019</v>
+      </c>
+      <c r="B2" s="28">
+        <v>4</v>
+      </c>
+      <c r="C2" s="28">
+        <v>25</v>
+      </c>
+      <c r="D2" s="26">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="25">
+        <v>44020</v>
+      </c>
+      <c r="B3" s="28">
+        <v>115</v>
+      </c>
+      <c r="C3" s="28">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="25">
+        <v>44021</v>
+      </c>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="25">
+        <v>44022</v>
+      </c>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="25">
+        <v>44023</v>
+      </c>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="36"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="25">
+        <v>44024</v>
+      </c>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="36"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="25">
+        <v>44025</v>
+      </c>
+      <c r="B8" s="28">
+        <v>145</v>
+      </c>
+      <c r="C8" s="50">
+        <v>132</v>
+      </c>
+      <c r="D8" s="28">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="25">
+        <v>44026</v>
+      </c>
+      <c r="B9" s="28">
+        <v>140</v>
+      </c>
+      <c r="C9" s="28">
+        <v>41</v>
+      </c>
+      <c r="D9" s="27"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="25">
+        <v>44027</v>
+      </c>
+      <c r="B10" s="28">
+        <v>45</v>
+      </c>
+      <c r="C10" s="26">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="25">
+        <v>44189</v>
+      </c>
+      <c r="B11" s="21">
+        <v>300</v>
+      </c>
+      <c r="C11" s="21">
+        <v>303</v>
+      </c>
+      <c r="D11" s="27">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="25">
+        <v>44190</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="21">
+        <v>316</v>
+      </c>
+      <c r="D12" s="52">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+      <c r="A13" s="25">
+        <v>44191</v>
+      </c>
+      <c r="B13" s="53">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="25">
+        <v>44192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="25">
+        <v>44193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="25">
+        <v>44194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="25">
+        <v>44195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="25">
+        <v>44196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="25">
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="25">
+        <v>44198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="25">
+        <v>44199</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="17" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A60059-9776-B34D-B54C-C4A089EF9F04}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="N16" activeCellId="1" sqref="A1 N16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>